<commit_message>
#219 add menu entry
</commit_message>
<xml_diff>
--- a/data/listCFPs.xlsx
+++ b/data/listCFPs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD174D6-0C22-4CA3-9960-61409DB70A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE9B63-BB13-4006-A287-5A9B038EFC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
   </bookViews>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}">
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3239,7 +3239,7 @@
         <v>12500</v>
       </c>
       <c r="G90" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#219 change table to make link clickable
</commit_message>
<xml_diff>
--- a/data/listCFPs.xlsx
+++ b/data/listCFPs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE9B63-BB13-4006-A287-5A9B038EFC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D02B0-3575-412F-86A6-301032CD58FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="276">
   <si>
     <t>Date</t>
   </si>
@@ -782,10 +782,85 @@
     <t>https://github.com/DeFiCh/dfips/issues/137</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>nb</t>
+  </si>
+  <si>
+    <t>05/2022</t>
+  </si>
+  <si>
+    <t>Moonrize - Reddit Posting Bot</t>
+  </si>
+  <si>
+    <t>Scott Rodgers &amp; Mathew Kovacs</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/138</t>
+  </si>
+  <si>
+    <t>dStocks Quickcheck</t>
+  </si>
+  <si>
+    <t>Robert S. aka robrevolver aka robbiraptor</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/143</t>
+  </si>
+  <si>
+    <t>Empowering more community members</t>
+  </si>
+  <si>
+    <t>Ruben Baas</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/146</t>
+  </si>
+  <si>
+    <t>The Jellyfish CFP: Sustaining Ocean Infrastructure Growth</t>
+  </si>
+  <si>
+    <t>Loh Fuxing - Jellyfish Maintainer</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/147</t>
+  </si>
+  <si>
+    <t>defichain-income.com implemented features</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/148</t>
+  </si>
+  <si>
+    <t>DeFiChain-Einstein.com</t>
+  </si>
+  <si>
+    <t>Lukas, Jan, Max und Simon</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/149</t>
+  </si>
+  <si>
+    <t>DeFiChain MediaPool</t>
+  </si>
+  <si>
+    <t>Inan Atalay</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/152</t>
+  </si>
+  <si>
+    <t>Providing liquidity on Pancakeswap in the BNB-DFI Pool</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/153</t>
+  </si>
+  <si>
+    <t>Bernd Mack and Andreas Lentz with mydefichain</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/154</t>
+  </si>
+  <si>
+    <t>Providing liquidity on Pancakeswap in the BUSD-DFI Pool</t>
   </si>
 </sst>
 </file>
@@ -1156,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B99" sqref="B91:B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1249,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3032,7 +3107,7 @@
         <v>2600</v>
       </c>
       <c r="G81" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3055,7 +3130,7 @@
         <v>1510</v>
       </c>
       <c r="G82" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3078,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="G83" t="s">
-        <v>249</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3101,7 +3176,7 @@
         <v>650</v>
       </c>
       <c r="G84" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3124,7 +3199,7 @@
         <v>4500</v>
       </c>
       <c r="G85" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3147,7 +3222,7 @@
         <v>189500</v>
       </c>
       <c r="G86" t="s">
-        <v>249</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3170,7 +3245,7 @@
         <v>1800</v>
       </c>
       <c r="G87" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3193,7 +3268,7 @@
         <v>2000</v>
       </c>
       <c r="G88" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3216,7 +3291,7 @@
         <v>30000</v>
       </c>
       <c r="G89" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3239,6 +3314,213 @@
         <v>12500</v>
       </c>
       <c r="G90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C91" t="s">
+        <v>251</v>
+      </c>
+      <c r="D91" t="s">
+        <v>252</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F91" s="3">
+        <v>8753</v>
+      </c>
+      <c r="G91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C92" t="s">
+        <v>254</v>
+      </c>
+      <c r="D92" t="s">
+        <v>255</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F92" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C93" t="s">
+        <v>257</v>
+      </c>
+      <c r="D93" t="s">
+        <v>258</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F93" s="3">
+        <v>22000</v>
+      </c>
+      <c r="G93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C94" t="s">
+        <v>260</v>
+      </c>
+      <c r="D94" t="s">
+        <v>261</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F94" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C95" t="s">
+        <v>263</v>
+      </c>
+      <c r="D95" t="s">
+        <v>25</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F95" s="3">
+        <v>12200</v>
+      </c>
+      <c r="G95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C96" t="s">
+        <v>265</v>
+      </c>
+      <c r="D96" t="s">
+        <v>266</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F96" s="3">
+        <v>3500</v>
+      </c>
+      <c r="G96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C97" t="s">
+        <v>268</v>
+      </c>
+      <c r="D97" t="s">
+        <v>269</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F97" s="3">
+        <v>18000</v>
+      </c>
+      <c r="G97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C98" t="s">
+        <v>271</v>
+      </c>
+      <c r="D98" t="s">
+        <v>273</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F98" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C99" t="s">
+        <v>275</v>
+      </c>
+      <c r="D99" t="s">
+        <v>273</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F99" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G99" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3336,8 +3618,17 @@
     <hyperlink ref="E88" r:id="rId89" xr:uid="{476AF6A0-7827-44A1-AF08-E6C1BC1B3077}"/>
     <hyperlink ref="E89" r:id="rId90" xr:uid="{F16F0DAF-F4E9-4E08-B703-4DB56F1C9E0E}"/>
     <hyperlink ref="E90" r:id="rId91" xr:uid="{8E9A1B90-CB09-428B-B1F8-7E192F9CD814}"/>
+    <hyperlink ref="E91" r:id="rId92" xr:uid="{C7D17E09-FA15-4DBB-B47C-577BAE7D4DF3}"/>
+    <hyperlink ref="E92" r:id="rId93" xr:uid="{9EF17F62-ACBE-450C-B473-B35808CE92E5}"/>
+    <hyperlink ref="E93" r:id="rId94" xr:uid="{7D4697E2-1554-42D5-BBBF-E59F07022D2F}"/>
+    <hyperlink ref="E94" r:id="rId95" xr:uid="{48E1253A-6742-48B9-8FFF-CC000C5FD37F}"/>
+    <hyperlink ref="E95" r:id="rId96" xr:uid="{66229A99-8586-4F0F-99AB-CBFA4D270756}"/>
+    <hyperlink ref="E96" r:id="rId97" xr:uid="{C2835CCD-F6BE-47F7-BFC6-8242CBFFEF46}"/>
+    <hyperlink ref="E97" r:id="rId98" xr:uid="{EB8E53C4-90E1-488A-BDC5-89DDE1583876}"/>
+    <hyperlink ref="E98" r:id="rId99" xr:uid="{77111824-D7DD-4F10-9B5D-F9BC43A1F55B}"/>
+    <hyperlink ref="E99" r:id="rId100" xr:uid="{6DC989BB-3DAC-44C5-A4BC-F7D6AD4332B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId92"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId101"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#254 adapt CFP evaluation
</commit_message>
<xml_diff>
--- a/data/listCFPs.xlsx
+++ b/data/listCFPs.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D02B0-3575-412F-86A6-301032CD58FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A686FAE6-894A-42FF-8E95-775FE7A556FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$117</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="379">
   <si>
     <t>Date</t>
   </si>
@@ -861,6 +864,315 @@
   </si>
   <si>
     <t>Providing liquidity on Pancakeswap in the BUSD-DFI Pool</t>
+  </si>
+  <si>
+    <t>07/2022</t>
+  </si>
+  <si>
+    <t>Pond, decentralize Ocean API and run it everywhere</t>
+  </si>
+  <si>
+    <t>Christian Sandrini, Oussama Ben Lagha</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/168</t>
+  </si>
+  <si>
+    <t>Development of a Wallet Monitoring System</t>
+  </si>
+  <si>
+    <t>Benjamin Bockmühl, Danny Blau, Elmar Lohe</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/169</t>
+  </si>
+  <si>
+    <t>Improvement and maintenance of DeFiChain-Analytics</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/171</t>
+  </si>
+  <si>
+    <t>saiive.live Infrastructure funding till end of year</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/172</t>
+  </si>
+  <si>
+    <t>dSEA - the NFT marketplace for DeFiChain</t>
+  </si>
+  <si>
+    <t>DeFiChainNFTs &amp; Team</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/173</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/174</t>
+  </si>
+  <si>
+    <t>Cashflow Butler - cashflow for everyone without crypto assets</t>
+  </si>
+  <si>
+    <t>Igor Shelkovenkov and Sebastian Lang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeFiChain-Cockpit - everything under control </t>
+  </si>
+  <si>
+    <t>Much &amp; Erich</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/175</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/176</t>
+  </si>
+  <si>
+    <t>Sharing is caring - DeFiChain Wiki Updates</t>
+  </si>
+  <si>
+    <t>Kassius84</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/177</t>
+  </si>
+  <si>
+    <t>Vault-maxi v2 and command center</t>
+  </si>
+  <si>
+    <t>Kuegi and Krysh</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/178</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/179</t>
+  </si>
+  <si>
+    <t>Matthias Nagele and Mirko Riedel</t>
+  </si>
+  <si>
+    <t>dSTOCKS.io - Trading wallet for synthetic assets</t>
+  </si>
+  <si>
+    <t>APOLLO MISSION - TRADE SHOWS</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/180</t>
+  </si>
+  <si>
+    <t>APOLLO MISSION - BRAND AWARENESS CAMPAIGN</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/181</t>
+  </si>
+  <si>
+    <t>JELLYWALLET FINAL CFP</t>
+  </si>
+  <si>
+    <t>DeFiChain Accelerator x Santiago Sabater</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/182</t>
+  </si>
+  <si>
+    <t>DeFiChain-Wizard - Automation for mass adoption</t>
+  </si>
+  <si>
+    <t>Sascha Sambale, Benjamin Bockmühl, Tim Gaggstatter, Sven Igl, Dario Leunig, Philip Lankes, Kevin Söll, Goran Amin</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/183</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/185</t>
+  </si>
+  <si>
+    <t>Jan &amp; Lukas</t>
+  </si>
+  <si>
+    <t>DeFiChain Community Explorer - An alternative explorer</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/186</t>
+  </si>
+  <si>
+    <t>U-Zyn</t>
+  </si>
+  <si>
+    <t>Liquidity mining reward for DFI ERC20 pairs at Uniswap</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/187</t>
+  </si>
+  <si>
+    <t>Decentralize DeFiChain Ocean</t>
+  </si>
+  <si>
+    <t>Expansion to the Russian Community</t>
+  </si>
+  <si>
+    <t>Vitali Gengel</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/188</t>
+  </si>
+  <si>
+    <t>08/2022</t>
+  </si>
+  <si>
+    <t>For moderation and technical improvement of the Telegram group: Crypto Steuern DACH</t>
+  </si>
+  <si>
+    <t>Johann Schlegel, Mark A., Karsten Salomon, Jascha und Steve K</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/192</t>
+  </si>
+  <si>
+    <t>Chain.report - Complete DeFiChain tax integration</t>
+  </si>
+  <si>
+    <t>Dr. Florian Lindner</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/193</t>
+  </si>
+  <si>
+    <t>Animated series for the DefiChain</t>
+  </si>
+  <si>
+    <t>Alperen Kocoglu</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/194</t>
+  </si>
+  <si>
+    <t>Hackathon for DeFi Meta Chain</t>
+  </si>
+  <si>
+    <t>Kong Yu Ning</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/197</t>
+  </si>
+  <si>
+    <t>International Staking Provider</t>
+  </si>
+  <si>
+    <t>Jonas Surmann</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/200</t>
+  </si>
+  <si>
+    <t>DeFiChain Italia - Italian Community Expansion</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/202</t>
+  </si>
+  <si>
+    <t>DefiChain YouTube Italian formats - ITA DeFiChain News Show + Video Tutorial</t>
+  </si>
+  <si>
+    <t>Angelo Castiglione &amp; Matteo Scalvini</t>
+  </si>
+  <si>
+    <t>Andrea Corsi, Simone Fontanesi</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/203</t>
+  </si>
+  <si>
+    <t>DefiChain Swiss Army Knife - The Ultimate multi-tool for daily activities</t>
+  </si>
+  <si>
+    <t>Ouss Benlagha</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/204</t>
+  </si>
+  <si>
+    <t>Top 10 Exchange Listing</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/205</t>
+  </si>
+  <si>
+    <t>Additional Trade Show Smartcon</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/206</t>
+  </si>
+  <si>
+    <t>Learn &amp; Earn Execution</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/207</t>
+  </si>
+  <si>
+    <t>DeFiChain Lottery Pot</t>
+  </si>
+  <si>
+    <t>Adrian, Christian</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/208</t>
+  </si>
+  <si>
+    <t>Historic Defichain Data, A Powerful Explorer, Correct Tax Reports (no-one has them) and Public Free API for Everyone</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/209</t>
+  </si>
+  <si>
+    <t>Economical Simulation Framework to Predict Effects of Consensus Changes on the Ecosystem</t>
+  </si>
+  <si>
+    <t>Kügi, Chris, Dr. Daniel Cagara</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/210</t>
+  </si>
+  <si>
+    <t>DefiCFP.org - cfp-tracking website</t>
+  </si>
+  <si>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/213</t>
+  </si>
+  <si>
+    <t>Nils Pfannkuchen, Manu Voss, Aleksandar Jovanovic, Tilman Kieselbach</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/214</t>
+  </si>
+  <si>
+    <t>DFSneo - a full custody brokerage mobile application for dAssets on DeFiChain</t>
+  </si>
+  <si>
+    <t>Auto-compounder &amp; Automated Delta Neutral Strategy to attract TVL &amp; help repeg DUSD</t>
+  </si>
+  <si>
+    <t>Aperture Finance, McDavid Stoddard</t>
+  </si>
+  <si>
+    <t>DeFiChain Captain - JellyfishSDK integration and performances improvements</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/217</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/216</t>
+  </si>
+  <si>
+    <t>Continue DFI rewards on BSC DFI-BNB pool on BSC/ACSI.finance</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/215</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B99" sqref="B91:B99"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2591,7 @@
         <v>20000</v>
       </c>
       <c r="G45" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3061,7 +3373,7 @@
         <v>25000</v>
       </c>
       <c r="G79" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3524,7 +3836,882 @@
         <v>10</v>
       </c>
     </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D100" t="s">
+        <v>278</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F100" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C101" t="s">
+        <v>280</v>
+      </c>
+      <c r="D101" t="s">
+        <v>281</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F101" s="3">
+        <v>28000</v>
+      </c>
+      <c r="G101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C102" t="s">
+        <v>283</v>
+      </c>
+      <c r="D102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F102" s="3">
+        <v>25000</v>
+      </c>
+      <c r="G102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C103" t="s">
+        <v>285</v>
+      </c>
+      <c r="D103" t="s">
+        <v>40</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F103" s="3">
+        <v>6000</v>
+      </c>
+      <c r="G103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C104" t="s">
+        <v>287</v>
+      </c>
+      <c r="D104" t="s">
+        <v>288</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F104" s="3">
+        <v>26300</v>
+      </c>
+      <c r="G104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C105" t="s">
+        <v>291</v>
+      </c>
+      <c r="D105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F105" s="3">
+        <v>175000</v>
+      </c>
+      <c r="G105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C106" t="s">
+        <v>293</v>
+      </c>
+      <c r="D106" t="s">
+        <v>294</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F106" s="3">
+        <v>45000</v>
+      </c>
+      <c r="G106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C107" t="s">
+        <v>92</v>
+      </c>
+      <c r="D107" t="s">
+        <v>90</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F107" s="3">
+        <v>41250</v>
+      </c>
+      <c r="G107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C108" t="s">
+        <v>297</v>
+      </c>
+      <c r="D108" t="s">
+        <v>298</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F108" s="3">
+        <v>3000</v>
+      </c>
+      <c r="G108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C109" t="s">
+        <v>300</v>
+      </c>
+      <c r="D109" t="s">
+        <v>301</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F109" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C110" t="s">
+        <v>305</v>
+      </c>
+      <c r="D110" t="s">
+        <v>304</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F110" s="3">
+        <v>85000</v>
+      </c>
+      <c r="G110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C111" t="s">
+        <v>306</v>
+      </c>
+      <c r="D111" t="s">
+        <v>121</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F111" s="3">
+        <v>132278</v>
+      </c>
+      <c r="G111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C112" t="s">
+        <v>308</v>
+      </c>
+      <c r="D112" t="s">
+        <v>121</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F112" s="3">
+        <v>281250</v>
+      </c>
+      <c r="G112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C113" t="s">
+        <v>310</v>
+      </c>
+      <c r="D113" t="s">
+        <v>311</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F113" s="3">
+        <v>168975</v>
+      </c>
+      <c r="G113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C114" t="s">
+        <v>313</v>
+      </c>
+      <c r="D114" t="s">
+        <v>314</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F114" s="3">
+        <v>42000</v>
+      </c>
+      <c r="G114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C115" t="s">
+        <v>318</v>
+      </c>
+      <c r="D115" t="s">
+        <v>317</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F115" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G115" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C116" t="s">
+        <v>321</v>
+      </c>
+      <c r="D116" t="s">
+        <v>320</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F116" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C117" t="s">
+        <v>323</v>
+      </c>
+      <c r="D117" t="s">
+        <v>273</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F117" s="3">
+        <v>8000</v>
+      </c>
+      <c r="G117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C118" t="s">
+        <v>324</v>
+      </c>
+      <c r="D118" t="s">
+        <v>325</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F118" s="3">
+        <v>40000</v>
+      </c>
+      <c r="G118" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C119" t="s">
+        <v>328</v>
+      </c>
+      <c r="D119" t="s">
+        <v>329</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F119" s="3">
+        <v>7860</v>
+      </c>
+      <c r="G119" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C120" t="s">
+        <v>331</v>
+      </c>
+      <c r="D120" t="s">
+        <v>332</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F120" s="3">
+        <v>115000</v>
+      </c>
+      <c r="G120" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C121" t="s">
+        <v>334</v>
+      </c>
+      <c r="D121" t="s">
+        <v>335</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F121" s="3">
+        <v>7000</v>
+      </c>
+      <c r="G121" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C122" t="s">
+        <v>337</v>
+      </c>
+      <c r="D122" t="s">
+        <v>338</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F122" s="3">
+        <v>350000</v>
+      </c>
+      <c r="G122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C123" t="s">
+        <v>340</v>
+      </c>
+      <c r="D123" t="s">
+        <v>341</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="F123" s="3">
+        <v>300000</v>
+      </c>
+      <c r="G123" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C124" t="s">
+        <v>343</v>
+      </c>
+      <c r="D124" t="s">
+        <v>347</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F124" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G124" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C125" t="s">
+        <v>345</v>
+      </c>
+      <c r="D125" t="s">
+        <v>346</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F125" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C126" t="s">
+        <v>349</v>
+      </c>
+      <c r="D126" t="s">
+        <v>350</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F126" s="3">
+        <v>15000</v>
+      </c>
+      <c r="G126" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C127" t="s">
+        <v>352</v>
+      </c>
+      <c r="D127" t="s">
+        <v>121</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F127" s="3">
+        <v>566772</v>
+      </c>
+      <c r="G127" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C128" t="s">
+        <v>354</v>
+      </c>
+      <c r="D128" t="s">
+        <v>121</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F128" s="3">
+        <v>27057</v>
+      </c>
+      <c r="G128" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C129" t="s">
+        <v>356</v>
+      </c>
+      <c r="D129" t="s">
+        <v>121</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F129" s="3">
+        <v>512658</v>
+      </c>
+      <c r="G129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C130" t="s">
+        <v>358</v>
+      </c>
+      <c r="D130" t="s">
+        <v>359</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F130" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C131" t="s">
+        <v>361</v>
+      </c>
+      <c r="D131" t="s">
+        <v>165</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F131" s="3">
+        <v>80000</v>
+      </c>
+      <c r="G131" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C132" t="s">
+        <v>363</v>
+      </c>
+      <c r="D132" t="s">
+        <v>364</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F132" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G132" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C133" t="s">
+        <v>366</v>
+      </c>
+      <c r="D133" t="s">
+        <v>367</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F133" s="3">
+        <v>39000</v>
+      </c>
+      <c r="G133" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C134" t="s">
+        <v>371</v>
+      </c>
+      <c r="D134" t="s">
+        <v>369</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F134" s="3">
+        <v>682000</v>
+      </c>
+      <c r="G134" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C135" t="s">
+        <v>372</v>
+      </c>
+      <c r="D135" t="s">
+        <v>373</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F135" s="3">
+        <v>75000</v>
+      </c>
+      <c r="G135" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C136" t="s">
+        <v>374</v>
+      </c>
+      <c r="D136" t="s">
+        <v>79</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F136" s="3">
+        <v>5100</v>
+      </c>
+      <c r="G136" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C137" t="s">
+        <v>377</v>
+      </c>
+      <c r="D137" t="s">
+        <v>188</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F137" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G137" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G117" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{FC5D919E-892D-4355-8922-E9D23CE83DC6}"/>
@@ -3627,8 +4814,46 @@
     <hyperlink ref="E97" r:id="rId98" xr:uid="{EB8E53C4-90E1-488A-BDC5-89DDE1583876}"/>
     <hyperlink ref="E98" r:id="rId99" xr:uid="{77111824-D7DD-4F10-9B5D-F9BC43A1F55B}"/>
     <hyperlink ref="E99" r:id="rId100" xr:uid="{6DC989BB-3DAC-44C5-A4BC-F7D6AD4332B1}"/>
+    <hyperlink ref="E100" r:id="rId101" xr:uid="{9442BD4C-D52B-40BA-8799-710AD7C39BA5}"/>
+    <hyperlink ref="E101" r:id="rId102" xr:uid="{AAB08E27-075A-4B07-87AA-599C37176569}"/>
+    <hyperlink ref="E102" r:id="rId103" xr:uid="{9F9926F8-9171-43EF-9FCD-8F120150FA53}"/>
+    <hyperlink ref="E103" r:id="rId104" xr:uid="{BB15246C-812B-4F8F-A9CF-2DE68A6AEBFC}"/>
+    <hyperlink ref="E104" r:id="rId105" xr:uid="{A26A0B1B-5EC6-485C-91C4-B28EF9FA9791}"/>
+    <hyperlink ref="E105" r:id="rId106" xr:uid="{C84F0309-8B48-495E-958A-902BB08AE6D9}"/>
+    <hyperlink ref="E106" r:id="rId107" xr:uid="{EAC4CC32-FDAF-4A42-A558-38A33006E214}"/>
+    <hyperlink ref="E107" r:id="rId108" xr:uid="{1C819B87-0DF0-4F85-BFCF-36EC08440ECB}"/>
+    <hyperlink ref="E108" r:id="rId109" xr:uid="{64303ED8-F602-48D5-86F8-689ADE5D299C}"/>
+    <hyperlink ref="E109" r:id="rId110" xr:uid="{D6159866-BA33-4CF7-A4C2-578DD3D86495}"/>
+    <hyperlink ref="E110" r:id="rId111" xr:uid="{B6C252DC-847B-4F2D-9CB5-3FBDE96305EF}"/>
+    <hyperlink ref="E111" r:id="rId112" xr:uid="{22569C6E-453E-4E0C-8E5C-519B7B3DA56B}"/>
+    <hyperlink ref="E112" r:id="rId113" xr:uid="{F069991F-F580-4433-98C5-1FD014B8D750}"/>
+    <hyperlink ref="E113" r:id="rId114" xr:uid="{E383110E-A944-476C-AA9E-3829BD860BF0}"/>
+    <hyperlink ref="E114" r:id="rId115" xr:uid="{25F1078E-9688-4F01-95ED-9F5D7CA80703}"/>
+    <hyperlink ref="E115" r:id="rId116" xr:uid="{1E488C26-7CB7-416D-AFA4-A192CF69CD9A}"/>
+    <hyperlink ref="E116" r:id="rId117" xr:uid="{7E8A3660-ECFC-4674-9A70-D9084A0441F7}"/>
+    <hyperlink ref="E117" r:id="rId118" xr:uid="{E17DDEC3-1AA0-4D3B-B3D3-9D6FA066ABFE}"/>
+    <hyperlink ref="E118" r:id="rId119" xr:uid="{C48EF062-5692-4BA5-B2E9-FAF9B8207A91}"/>
+    <hyperlink ref="E119" r:id="rId120" xr:uid="{CEAE9337-BA7F-4BAA-A7B9-532E8DA26EDE}"/>
+    <hyperlink ref="E120" r:id="rId121" xr:uid="{AA440D85-17F6-414B-B6E6-66C59202B259}"/>
+    <hyperlink ref="E121" r:id="rId122" xr:uid="{892454E6-6877-470F-B9B5-653A05C8EFC6}"/>
+    <hyperlink ref="E122" r:id="rId123" xr:uid="{87191D92-0B59-4A8D-9E5E-9074C839F0DC}"/>
+    <hyperlink ref="E123" r:id="rId124" xr:uid="{63B62B15-E143-4079-A0D5-9A714D7B19C4}"/>
+    <hyperlink ref="E124" r:id="rId125" xr:uid="{CDE5877D-6893-4AA5-857F-529C60790D53}"/>
+    <hyperlink ref="E125" r:id="rId126" xr:uid="{2EEAFCC3-74D6-4538-988A-0641B47D2704}"/>
+    <hyperlink ref="E126" r:id="rId127" xr:uid="{7B2DF56B-D820-473C-B382-18D8015DC19B}"/>
+    <hyperlink ref="E127" r:id="rId128" xr:uid="{B0C6E287-D4B4-4F7C-8CD8-1A8AFF63515A}"/>
+    <hyperlink ref="E128" r:id="rId129" xr:uid="{08C9C9A1-7F69-46D2-89BE-736B718E49E5}"/>
+    <hyperlink ref="E129" r:id="rId130" xr:uid="{E02AC3A6-EC12-4822-AD79-C61062BA67C8}"/>
+    <hyperlink ref="E130" r:id="rId131" xr:uid="{DA2DB96F-353E-4A86-8BB4-94015D3E4BE9}"/>
+    <hyperlink ref="E131" r:id="rId132" xr:uid="{E39B0C46-7760-45E5-B5C0-E5B7E58863A0}"/>
+    <hyperlink ref="E132" r:id="rId133" xr:uid="{C697A4F4-5E4C-4093-A075-50EEDC287737}"/>
+    <hyperlink ref="E133" r:id="rId134" xr:uid="{77B9A982-6FFC-48F0-B0D1-EE8D30FB53CA}"/>
+    <hyperlink ref="E134" r:id="rId135" xr:uid="{F85885A0-E450-41DB-BF5D-7868F82A833C}"/>
+    <hyperlink ref="E136" r:id="rId136" xr:uid="{9B8FCE05-1613-474E-8375-BAB419F9D222}"/>
+    <hyperlink ref="E135" r:id="rId137" xr:uid="{359CAEF5-9AD7-4851-B298-EA16EAA6EDB1}"/>
+    <hyperlink ref="E137" r:id="rId138" xr:uid="{B50B84CD-22F8-45AD-8511-E2A447448805}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId101"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId139"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#266 add CFP results to list
</commit_message>
<xml_diff>
--- a/data/listCFPs.xlsx
+++ b/data/listCFPs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A686FAE6-894A-42FF-8E95-775FE7A556FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F71E7A-AC03-47F8-A0BA-EC74740AC427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="414">
   <si>
     <t>Date</t>
   </si>
@@ -1173,6 +1173,111 @@
   </si>
   <si>
     <t>https://github.com/DeFiCh/dfips/issues/215</t>
+  </si>
+  <si>
+    <t>11/2022</t>
+  </si>
+  <si>
+    <t>DFI earnings automation: defichain-compound</t>
+  </si>
+  <si>
+    <t>Luzian Scherrer</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/220</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/221</t>
+  </si>
+  <si>
+    <t>LauraL</t>
+  </si>
+  <si>
+    <t>DeFiChain CFPs &amp; DFIPs Dashboard</t>
+  </si>
+  <si>
+    <t>DeFi Meta Chain $100M Incubator Program</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/223</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/224</t>
+  </si>
+  <si>
+    <t>mydefichain Ocean Q4/2022</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/225</t>
+  </si>
+  <si>
+    <t>mydefichain Ocean Q1/2023</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/226</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/229</t>
+  </si>
+  <si>
+    <t>Bring DFI to the next level</t>
+  </si>
+  <si>
+    <t>Dominik &amp; Dwight from Make-it pro</t>
+  </si>
+  <si>
+    <t>DeFiChain Poker Nights</t>
+  </si>
+  <si>
+    <t>DeFiChainNFTs + Holy_Amanita</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/231</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/233</t>
+  </si>
+  <si>
+    <t>WalletWatcher - A mobile app to monitor all wallets which are important to you</t>
+  </si>
+  <si>
+    <t>Aleksandar Jovanovic, Tilman Kieselbach</t>
+  </si>
+  <si>
+    <t>DeFiChain Python Library II</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/234</t>
+  </si>
+  <si>
+    <t>DeFi-Seedfinder - Crowdinvesting on DeFiChain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nils, Manu, Aleks, Til</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/235</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/240</t>
+  </si>
+  <si>
+    <t>Telegram moderators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO for DEFICHAIN.COM </t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/242</t>
+  </si>
+  <si>
+    <t>Krypto-Sprungbrett &amp; dfidex.live by ChristophG</t>
+  </si>
+  <si>
+    <t>Michael from DeFiChain.Info</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/243</t>
   </si>
 </sst>
 </file>
@@ -1223,11 +1328,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1543,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4707,6 +4815,328 @@
         <v>20000</v>
       </c>
       <c r="G137" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C138" t="s">
+        <v>380</v>
+      </c>
+      <c r="D138" t="s">
+        <v>381</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F138" s="3">
+        <v>3569</v>
+      </c>
+      <c r="G138" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C139" t="s">
+        <v>385</v>
+      </c>
+      <c r="D139" t="s">
+        <v>384</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F139" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G139" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C140" t="s">
+        <v>386</v>
+      </c>
+      <c r="D140" t="s">
+        <v>338</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F140" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="G140" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C141" t="s">
+        <v>51</v>
+      </c>
+      <c r="D141" t="s">
+        <v>273</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F141" s="3">
+        <v>28500</v>
+      </c>
+      <c r="G141" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C142" t="s">
+        <v>389</v>
+      </c>
+      <c r="D142" t="s">
+        <v>273</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F142" s="3">
+        <v>9500</v>
+      </c>
+      <c r="G142" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C143" t="s">
+        <v>391</v>
+      </c>
+      <c r="D143" t="s">
+        <v>273</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F143" s="3">
+        <v>9500</v>
+      </c>
+      <c r="G143" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C144" t="s">
+        <v>394</v>
+      </c>
+      <c r="D144" t="s">
+        <v>395</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F144" s="3">
+        <v>375000</v>
+      </c>
+      <c r="G144" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C145" t="s">
+        <v>396</v>
+      </c>
+      <c r="D145" t="s">
+        <v>397</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="F145" s="3">
+        <v>3636</v>
+      </c>
+      <c r="G145" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C146" t="s">
+        <v>400</v>
+      </c>
+      <c r="D146" t="s">
+        <v>401</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F146" s="3">
+        <v>15000</v>
+      </c>
+      <c r="G146" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C147" t="s">
+        <v>402</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="F147" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G147" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C148" t="s">
+        <v>404</v>
+      </c>
+      <c r="D148" t="s">
+        <v>405</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F148" s="3">
+        <v>95000</v>
+      </c>
+      <c r="G148" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C149" t="s">
+        <v>92</v>
+      </c>
+      <c r="D149" t="s">
+        <v>408</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F149" s="3">
+        <v>52550</v>
+      </c>
+      <c r="G149" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>150</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C150" t="s">
+        <v>409</v>
+      </c>
+      <c r="D150" t="s">
+        <v>121</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F150" s="3">
+        <v>32960</v>
+      </c>
+      <c r="G150" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>151</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C151" t="s">
+        <v>411</v>
+      </c>
+      <c r="D151" t="s">
+        <v>412</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F151" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G151" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4852,8 +5282,22 @@
     <hyperlink ref="E136" r:id="rId136" xr:uid="{9B8FCE05-1613-474E-8375-BAB419F9D222}"/>
     <hyperlink ref="E135" r:id="rId137" xr:uid="{359CAEF5-9AD7-4851-B298-EA16EAA6EDB1}"/>
     <hyperlink ref="E137" r:id="rId138" xr:uid="{B50B84CD-22F8-45AD-8511-E2A447448805}"/>
+    <hyperlink ref="E138" r:id="rId139" xr:uid="{9B7B585E-B322-42A6-84D5-0DD94A63BD4F}"/>
+    <hyperlink ref="E139" r:id="rId140" xr:uid="{9B4728CC-A463-4FAB-947A-C6E90AC2F7C7}"/>
+    <hyperlink ref="E140" r:id="rId141" xr:uid="{9F243D43-469C-4DDB-9FBA-A6001B94C41B}"/>
+    <hyperlink ref="E141" r:id="rId142" xr:uid="{DAB59AFB-EC54-436C-910E-971B702A0FDA}"/>
+    <hyperlink ref="E142" r:id="rId143" xr:uid="{A145D6FA-808F-4DFE-84D7-DC17936A07CE}"/>
+    <hyperlink ref="E143" r:id="rId144" xr:uid="{ED62AE90-3D4F-4C88-A614-7425DC7C1A79}"/>
+    <hyperlink ref="E144" r:id="rId145" xr:uid="{E3E1A809-86DD-423A-9FF0-E0AC8B8BC4CE}"/>
+    <hyperlink ref="E145" r:id="rId146" xr:uid="{9E19EFF8-04CE-4EE2-9958-C72D9C0E6001}"/>
+    <hyperlink ref="E146" r:id="rId147" xr:uid="{7D132680-C6AB-4971-BEDB-133DEFFD4225}"/>
+    <hyperlink ref="E147" r:id="rId148" xr:uid="{98D21F59-B839-45CE-87C7-0D788D8BAB15}"/>
+    <hyperlink ref="E148" r:id="rId149" xr:uid="{E32040B4-AB09-4C4B-AEAD-8DBDFC1DE77A}"/>
+    <hyperlink ref="E149" r:id="rId150" xr:uid="{69F43550-3CBC-4204-9F1D-BE08F6ABD51C}"/>
+    <hyperlink ref="E150" r:id="rId151" xr:uid="{0B5AF68F-4328-4496-AF16-91AB6B0FBD8D}"/>
+    <hyperlink ref="E151" r:id="rId152" xr:uid="{AB1EF367-CFD7-40D5-BF41-42241748B0A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId139"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId153"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#295 update cfp list
</commit_message>
<xml_diff>
--- a/data/listCFPs.xlsx
+++ b/data/listCFPs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F71E7A-AC03-47F8-A0BA-EC74740AC427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C0625B-0B84-4CAD-985C-DE53F58E4AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
   </bookViews>
@@ -23,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="441">
   <si>
     <t>Date</t>
   </si>
@@ -1253,9 +1245,6 @@
     <t>DeFi-Seedfinder - Crowdinvesting on DeFiChain</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nils, Manu, Aleks, Til</t>
-  </si>
-  <si>
     <t>https://github.com/DeFiCh/dfips/issues/235</t>
   </si>
   <si>
@@ -1278,6 +1267,90 @@
   </si>
   <si>
     <t>https://github.com/DeFiCh/dfips/issues/243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeFiChainWiki </t>
+  </si>
+  <si>
+    <t>Joshua Kummer</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/10l6451/cfp_defichainwiki_9000_dfi/</t>
+  </si>
+  <si>
+    <t>,InTheMarket’’ Podcast</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/1051xfw/cfp_inthemarket_podcast</t>
+  </si>
+  <si>
+    <t>Patrick (Peddy)</t>
+  </si>
+  <si>
+    <t>Ongoing Investigation/Case Atomic Swap-dBTC Exploit on DeFiChain - Budget 2023</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/10wrrt2/cfp_ongoing_investigationcase_atomic_swapdbtc/</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/246</t>
+  </si>
+  <si>
+    <t>DeFiChain Epic, DeFiChain Accelerator</t>
+  </si>
+  <si>
+    <t>Sponsorship of the National Fighting Championship (NFC)</t>
+  </si>
+  <si>
+    <t>defichain-trader.com</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/10l35aj/cfp_defichaintradercom/</t>
+  </si>
+  <si>
+    <t>Ruben</t>
+  </si>
+  <si>
+    <t>Nils, Manu, Aleks, Til</t>
+  </si>
+  <si>
+    <t>Portfolio Optimisation with Modern Portfolio Theory</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/10x7jhn/cfp_portfolio_optimisation_with_modern_portfolio/</t>
+  </si>
+  <si>
+    <t>defichain-trader.com (Maintenance)</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/258</t>
+  </si>
+  <si>
+    <t>04/2023</t>
+  </si>
+  <si>
+    <t>02/2023</t>
+  </si>
+  <si>
+    <t>Appreciation of the work done by Kügi in the community in the last months</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/11fj7i5/cfp_appreciation_of_the_work_done_by_k%C3%BCgi_in_the/</t>
+  </si>
+  <si>
+    <t>Phigo</t>
+  </si>
+  <si>
+    <t>mydefichain-Ocean-2023</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/11g01xa/cfp_mydefichain_ocean_funding_2023_6850_dfi_per/</t>
+  </si>
+  <si>
+    <t>https://github.com/DeFiCh/dfips/issues/256</t>
   </si>
 </sst>
 </file>
@@ -1651,17 +1724,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}">
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G152" sqref="G152"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="119" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.7109375" customWidth="1"/>
     <col min="4" max="4" width="55.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="3"/>
@@ -5059,10 +5132,10 @@
         <v>404</v>
       </c>
       <c r="D148" t="s">
+        <v>427</v>
+      </c>
+      <c r="E148" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="F148" s="3">
         <v>95000</v>
@@ -5082,10 +5155,10 @@
         <v>92</v>
       </c>
       <c r="D149" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F149" s="3">
         <v>52550</v>
@@ -5102,13 +5175,13 @@
         <v>379</v>
       </c>
       <c r="C150" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D150" t="s">
         <v>121</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F150" s="3">
         <v>32960</v>
@@ -5125,19 +5198,249 @@
         <v>379</v>
       </c>
       <c r="C151" t="s">
+        <v>410</v>
+      </c>
+      <c r="D151" t="s">
         <v>411</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="F151" s="3">
         <v>5000</v>
       </c>
       <c r="G151" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>152</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C152" t="s">
+        <v>413</v>
+      </c>
+      <c r="D152" t="s">
+        <v>414</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="F152" s="3">
+        <v>9000</v>
+      </c>
+      <c r="G152" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>153</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C153" t="s">
+        <v>416</v>
+      </c>
+      <c r="D153" t="s">
+        <v>418</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F153" s="3">
+        <v>9000</v>
+      </c>
+      <c r="G153" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>154</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C154" t="s">
+        <v>419</v>
+      </c>
+      <c r="D154" t="s">
+        <v>212</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F154" s="3">
+        <v>200000</v>
+      </c>
+      <c r="G154" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C155" t="s">
+        <v>423</v>
+      </c>
+      <c r="D155" t="s">
+        <v>422</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="F155" s="3">
+        <v>500000</v>
+      </c>
+      <c r="G155" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>156</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C156" t="s">
+        <v>424</v>
+      </c>
+      <c r="D156" t="s">
+        <v>426</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="F156" s="3">
+        <v>110000</v>
+      </c>
+      <c r="G156" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>157</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C157" t="s">
+        <v>428</v>
+      </c>
+      <c r="D157" t="s">
+        <v>429</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="F157" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G157" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>158</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C158" t="s">
+        <v>431</v>
+      </c>
+      <c r="D158" t="s">
+        <v>426</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="F158" s="3">
+        <v>5400</v>
+      </c>
+      <c r="G158" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>159</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C159" t="s">
+        <v>435</v>
+      </c>
+      <c r="D159" t="s">
+        <v>437</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="F159" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G159" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>160</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C160" t="s">
+        <v>438</v>
+      </c>
+      <c r="D160" t="s">
+        <v>273</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F160" s="3">
+        <v>6850</v>
+      </c>
+      <c r="G160" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>161</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C161" t="s">
+        <v>377</v>
+      </c>
+      <c r="D161" t="s">
+        <v>188</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="F161" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G161" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -5296,8 +5599,18 @@
     <hyperlink ref="E149" r:id="rId150" xr:uid="{69F43550-3CBC-4204-9F1D-BE08F6ABD51C}"/>
     <hyperlink ref="E150" r:id="rId151" xr:uid="{0B5AF68F-4328-4496-AF16-91AB6B0FBD8D}"/>
     <hyperlink ref="E151" r:id="rId152" xr:uid="{AB1EF367-CFD7-40D5-BF41-42241748B0A1}"/>
+    <hyperlink ref="E152" r:id="rId153" xr:uid="{78E7AE0B-61EF-4B6B-B751-4FF6A8EEA8A2}"/>
+    <hyperlink ref="E153" r:id="rId154" xr:uid="{FB40D154-EC86-44FE-9938-6DE14AC69865}"/>
+    <hyperlink ref="E154" r:id="rId155" xr:uid="{05B2A674-A4A9-443E-9DED-B40741B52F6D}"/>
+    <hyperlink ref="E155" r:id="rId156" xr:uid="{3F91CE20-33FF-4F75-9128-603DFB95C318}"/>
+    <hyperlink ref="E156" r:id="rId157" xr:uid="{562201A6-9573-4030-9502-C4F815AC1564}"/>
+    <hyperlink ref="E157" r:id="rId158" xr:uid="{4FF4A3D5-053B-4875-A728-C7420BE43413}"/>
+    <hyperlink ref="E158" r:id="rId159" xr:uid="{510A23EF-8488-4B63-A386-31E9E27F1631}"/>
+    <hyperlink ref="E159" r:id="rId160" xr:uid="{1496DF5F-0458-4D3F-9B38-972FFB6C8FC5}"/>
+    <hyperlink ref="E160" r:id="rId161" xr:uid="{CDF416AF-E9E3-4750-A647-5CDFA9CF11BF}"/>
+    <hyperlink ref="E161" r:id="rId162" xr:uid="{75C7758B-4609-4A7D-83E8-F40DC794B37E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId153"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId163"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#300 update CFP list
</commit_message>
<xml_diff>
--- a/data/listCFPs.xlsx
+++ b/data/listCFPs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C0625B-0B84-4CAD-985C-DE53F58E4AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912C7E68-636C-4696-BED0-055354AB0532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AE1D34F0-3539-47C2-9FC6-EC55CC4BCD44}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="455">
   <si>
     <t>Date</t>
   </si>
@@ -1351,6 +1351,48 @@
   </si>
   <si>
     <t>https://github.com/DeFiCh/dfips/issues/256</t>
+  </si>
+  <si>
+    <t>06/2023</t>
+  </si>
+  <si>
+    <t>mydefichain Ocean 2023 Cycle-2</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/12qhhj5/mydefichain_ocean_2023_actual_cycle_round/</t>
+  </si>
+  <si>
+    <t>Telegram Moderators H1 2023</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/12rugem/telegram_moderators_h1_2023/</t>
+  </si>
+  <si>
+    <t>Integration of Yield Machine and Interest Rates on defichain-income.com</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/125s2s7/integration_of_yield_machine_and_interest_rates/</t>
+  </si>
+  <si>
+    <t>mydefichain-Ocean-2023-cycle-3</t>
+  </si>
+  <si>
+    <t>07/2023</t>
+  </si>
+  <si>
+    <t>mydefichain-Ocean-2023-cycle-4</t>
+  </si>
+  <si>
+    <t>09/2023</t>
+  </si>
+  <si>
+    <t>DeFiChain Turkey - On the Way to Becoming the Biggest Regional Community</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/defiblockchain/comments/1456fnx/cfp_defichain_turkey_on_the_way_to_becoming_the/</t>
+  </si>
+  <si>
+    <t>DeFiChain Turkey</t>
   </si>
 </sst>
 </file>
@@ -1724,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A9972-4C6E-4DF5-AA5B-3B2DAAC71C59}">
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5441,6 +5483,144 @@
       </c>
       <c r="G161" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>162</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C162" t="s">
+        <v>442</v>
+      </c>
+      <c r="D162" t="s">
+        <v>273</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F162" s="3">
+        <v>7500</v>
+      </c>
+      <c r="G162" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>163</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C163" t="s">
+        <v>444</v>
+      </c>
+      <c r="D163" t="s">
+        <v>407</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="F163" s="3">
+        <v>82750</v>
+      </c>
+      <c r="G163" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>164</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C164" t="s">
+        <v>446</v>
+      </c>
+      <c r="D164" t="s">
+        <v>25</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="F164" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G164" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>165</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C165" t="s">
+        <v>448</v>
+      </c>
+      <c r="D165" t="s">
+        <v>273</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F165" s="3">
+        <v>11000</v>
+      </c>
+      <c r="G165" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>166</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C166" t="s">
+        <v>450</v>
+      </c>
+      <c r="D166" t="s">
+        <v>273</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F166" s="3">
+        <v>11000</v>
+      </c>
+      <c r="G166" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>167</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C167" t="s">
+        <v>452</v>
+      </c>
+      <c r="D167" t="s">
+        <v>454</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="F167" s="3">
+        <v>45000</v>
+      </c>
+      <c r="G167" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5609,8 +5789,14 @@
     <hyperlink ref="E159" r:id="rId160" xr:uid="{1496DF5F-0458-4D3F-9B38-972FFB6C8FC5}"/>
     <hyperlink ref="E160" r:id="rId161" xr:uid="{CDF416AF-E9E3-4750-A647-5CDFA9CF11BF}"/>
     <hyperlink ref="E161" r:id="rId162" xr:uid="{75C7758B-4609-4A7D-83E8-F40DC794B37E}"/>
+    <hyperlink ref="E162" r:id="rId163" xr:uid="{9035EBAA-1322-4369-8E21-63CA3BF51FF8}"/>
+    <hyperlink ref="E163" r:id="rId164" xr:uid="{B597D993-A098-4D6B-968D-515731B9F7B2}"/>
+    <hyperlink ref="E164" r:id="rId165" xr:uid="{B0378C5F-A285-4377-9D11-D75593FFA54A}"/>
+    <hyperlink ref="E165" r:id="rId166" xr:uid="{0E6FAF34-580A-4904-9D70-95D6B400EAE0}"/>
+    <hyperlink ref="E166" r:id="rId167" xr:uid="{AD3DB981-C8AF-49AF-8907-7B3473CA5915}"/>
+    <hyperlink ref="E167" r:id="rId168" xr:uid="{A214B730-D33F-4B88-BF3D-676FCE2069FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId163"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId169"/>
 </worksheet>
 </file>
</xml_diff>